<commit_message>
fix: Fixed column values
</commit_message>
<xml_diff>
--- a/tests/test_files/handlers/reports/report.xlsx
+++ b/tests/test_files/handlers/reports/report.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="true" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tenencia" sheetId="1" r:id="rId1"/>
+    <sheet name="Variacion - Retorno" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>DateRequested</t>
   </si>
@@ -35,6 +36,9 @@
   </si>
   <si>
     <t>2024-08-03</t>
+  </si>
+  <si>
+    <t>0.000000</t>
   </si>
 </sst>
 </file>
@@ -340,7 +344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -386,4 +390,55 @@
     <mergeCell ref="B1:B1"/>
   </mergeCells>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="true" workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:B1"/>
+  </mergeCells>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Added liquidaciones and boletos
</commit_message>
<xml_diff>
--- a/tests/test_files/handlers/reports/report.xlsx
+++ b/tests/test_files/handlers/reports/report.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>DateRequested</t>
+    <t>Fecha</t>
   </si>
   <si>
     <t>S31E5</t>
@@ -29,7 +29,7 @@
     <t>2024-08-01</t>
   </si>
   <si>
-    <t>768873866.640000</t>
+    <t>768873866.64</t>
   </si>
   <si>
     <t>2024-08-02</t>
@@ -45,20 +45,61 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b val="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFADD8E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4682B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -73,8 +114,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="false">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="false">
+      <alignment/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -347,22 +400,35 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col max="1" min="1" style="1" width="9.140625"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" s="4" customFormat="true">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
@@ -370,7 +436,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
@@ -378,7 +444,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
@@ -398,22 +464,35 @@
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
+  <cols>
+    <col max="1" min="1" style="1" width="9.140625"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" s="4" customFormat="true">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
@@ -421,7 +500,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
@@ -429,7 +508,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">

</xml_diff>

<commit_message>
feat: Added logo on report pdf
</commit_message>
<xml_diff>
--- a/tests/test_files/handlers/reports/report.xlsx
+++ b/tests/test_files/handlers/reports/report.xlsx
@@ -4,31 +4,56 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="true" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tenencia" sheetId="1" r:id="rId1"/>
-    <sheet name="Variacion - Retorno" sheetId="2" r:id="rId5"/>
+    <sheet name="Retorno" sheetId="2" r:id="rId5"/>
+    <sheet name="Referencias" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Fecha</t>
   </si>
   <si>
+    <t>YMCQO</t>
+  </si>
+  <si>
+    <t>DGCU2</t>
+  </si>
+  <si>
+    <t>PBR</t>
+  </si>
+  <si>
     <t>S31E5</t>
   </si>
   <si>
+    <t>RENTA VARIABLE</t>
+  </si>
+  <si>
     <t>TASA FIJA</t>
   </si>
   <si>
+    <t>ON HARD DOLLAR</t>
+  </si>
+  <si>
     <t>2024-08-01</t>
   </si>
   <si>
+    <t>222222222.64</t>
+  </si>
+  <si>
+    <t>9999999.64</t>
+  </si>
+  <si>
+    <t>1111111111.64</t>
+  </si>
+  <si>
     <t>768873866.64</t>
   </si>
   <si>
@@ -38,7 +63,16 @@
     <t>2024-08-03</t>
   </si>
   <si>
-    <t>0.000000</t>
+    <t>-</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>Tasa de interés de préstamos por adelantos en cuenta corriente</t>
+  </si>
+  <si>
+    <t>Variables de Referencia</t>
   </si>
 </sst>
 </file>
@@ -407,11 +441,15 @@
     <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
       <c r="H1" s="2"/>
@@ -426,39 +464,183 @@
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:E1"/>
     <mergeCell ref="B1:B1"/>
   </mergeCells>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col max="1" min="1" style="1" width="9.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" s="4" customFormat="true">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:E1"/>
+  </mergeCells>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -471,7 +653,7 @@
     <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="2"/>
@@ -488,31 +670,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Added caching layer
</commit_message>
<xml_diff>
--- a/tests/test_files/handlers/reports/report.xlsx
+++ b/tests/test_files/handlers/reports/report.xlsx
@@ -33,13 +33,13 @@
     <t>S31E5</t>
   </si>
   <si>
+    <t>ON HARD DOLLAR</t>
+  </si>
+  <si>
     <t>RENTA VARIABLE</t>
   </si>
   <si>
     <t>TASA FIJA</t>
-  </si>
-  <si>
-    <t>ON HARD DOLLAR</t>
   </si>
   <si>
     <t>2024-08-01</t>
@@ -441,14 +441,14 @@
     <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
@@ -527,9 +527,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="B1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E1"/>
-    <mergeCell ref="B1:B1"/>
   </mergeCells>
 </worksheet>
 </file>
@@ -547,14 +547,14 @@
     <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
@@ -633,9 +633,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E1"/>
     <mergeCell ref="B1:B1"/>
+    <mergeCell ref="C1:D1"/>
   </mergeCells>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fix: Fixed issue with intrumentos
</commit_message>
<xml_diff>
--- a/tests/test_files/handlers/reports/report.xlsx
+++ b/tests/test_files/handlers/reports/report.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="true" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Tenencia" sheetId="1" r:id="rId1"/>
     <sheet name="Tenencia - Barras" sheetId="2" r:id="rId5"/>
-    <sheet name="Tenencia_Porcentaje" sheetId="3" r:id="rId6"/>
-    <sheet name="Tenencia_Porcentaje - Barras" sheetId="4" r:id="rId7"/>
-    <sheet name="Retorno" sheetId="5" r:id="rId8"/>
-    <sheet name="Retorno - Barras" sheetId="6" r:id="rId9"/>
-    <sheet name="Referencias" sheetId="7" r:id="rId10"/>
-    <sheet name="Referencias - Barras" sheetId="8" r:id="rId11"/>
+    <sheet name="Tenencia - Pie Chart" sheetId="3" r:id="rId6"/>
+    <sheet name="Tenencia_Porcentaje" sheetId="4" r:id="rId7"/>
+    <sheet name="Tenencia_Porcentaje - Barras" sheetId="5" r:id="rId8"/>
+    <sheet name="Retorno" sheetId="6" r:id="rId9"/>
+    <sheet name="Retorno - Barras" sheetId="7" r:id="rId10"/>
+    <sheet name="Referencias" sheetId="8" r:id="rId11"/>
+    <sheet name="Referencias - Barras" sheetId="9" r:id="rId12"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -41,9 +42,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
     <t>ON HARD DOLLAR</t>
   </si>
   <si>
@@ -51,6 +49,9 @@
   </si>
   <si>
     <t>TASA FIJA</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
   <si>
     <t>2024-08-01</t>
@@ -516,6 +517,135 @@
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
               </a:rPr>
+              <a:t>Tenencia</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="en-US"/>
+          </a:p>
+        </rich>
+      </tx>
+      <overlay val="0"/>
+      <spPr/>
+      <txPr>
+        <a:bodyPr anchorCtr="false" rot="0" spcFirstLastPara="false"/>
+        <a:p/>
+      </txPr>
+    </title>
+    <view3D>
+      <rotX val="0"/>
+      <rotY val="0"/>
+      <rAngAx val="0"/>
+      <perspective val="0"/>
+    </view3D>
+    <floor>
+      <thickness val="0"/>
+    </floor>
+    <sideWall>
+      <thickness val="0"/>
+    </sideWall>
+    <backWall>
+      <thickness val="0"/>
+    </backWall>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>Tenencia</f>
+            </strRef>
+          </tx>
+          <dPt>
+            <idx val="0"/>
+            <bubble3D val="0"/>
+            <spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln cap="rnd" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </spPr>
+          </dPt>
+          <dLbls>
+            <showLegendKey val="0"/>
+            <showVal val="1"/>
+            <showCatName val="1"/>
+            <showSerName val="0"/>
+            <showPercent val="1"/>
+            <showBubbleSize val="0"/>
+            <showLeaderLines val="0"/>
+          </dLbls>
+          <invertIfNegative val="0"/>
+          <cat>
+            <strRef>
+              <f>Tenencia!$B$2:$E$2</f>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>Tenencia!$B$5:$E$5</f>
+            </numRef>
+          </val>
+          <smooth val="0"/>
+        </ser>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+      <overlay val="0"/>
+    </legend>
+    <plotVisOnly val="0"/>
+    <dispBlanksAs val="gap"/>
+    <showDLblsOverMax val="0"/>
+  </chart>
+  <spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </a:ln>
+  </spPr>
+  <printSettings>
+    <pageMargins b="0.75" footer="0.3" header="0.3" l="0.7" r="0.7" t="0.7"/>
+  </printSettings>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <date1904 val="0"/>
+  <lang val="en-US"/>
+  <roundedCorners val="0"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr anchorCtr="false" rot="0" spcFirstLastPara="false"/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="false" baseline="0" i="false" kern="0" spc="0"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="true" baseline="0" i="false" kern="0" spc="0" sz="3500">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t>Tenencia_Porcentaje</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" altLang="en-US"/>
@@ -825,7 +955,7 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <date1904 val="0"/>
   <lang val="en-US"/>
@@ -1154,7 +1284,7 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <date1904 val="0"/>
   <lang val="en-US"/>
@@ -1403,15 +1533,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1469,6 +1599,41 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 2" descr=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="false" fPrintsWithSheet="true"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1773,17 +1938,17 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
@@ -1856,27 +2021,27 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>222222222.64</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>9999999.64</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1111111111.64</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>768873866.64</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>2112207200.56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="F1:F1"/>
     <mergeCell ref="B1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E1"/>
+    <mergeCell ref="F1:F1"/>
   </mergeCells>
 </worksheet>
 </file>
@@ -1910,127 +2075,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <cols>
-    <col max="1" min="1" style="2" width="9.140625"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="4"/>
-    </row>
-    <row r="2" s="5" customFormat="true">
-      <c r="A2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0.105209</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.004734</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.526043</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.364014</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2112207200.56</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.105209</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.004734</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.526043</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.364014</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2112207200.56</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:E1"/>
-    <mergeCell ref="F1:F1"/>
-  </mergeCells>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2058,7 +2102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2071,17 +2115,17 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
@@ -2113,73 +2157,73 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
+      <c r="B3" s="1">
+        <v>0.105209</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.004734</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.526043</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.364014</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2112207200.56</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
+      <c r="B4" s="1">
+        <v>0.105209</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.004734</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.526043</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.364014</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2112207200.56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
+      <c r="B5" s="1">
+        <v>0.105209</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.004734</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.526043</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.364014</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2112207200.56</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E1"/>
     <mergeCell ref="F1:F1"/>
+    <mergeCell ref="B1:B1"/>
   </mergeCells>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2207,7 +2251,156 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col max="1" min="1" style="2" width="9.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" s="5" customFormat="true">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:E1"/>
+    <mergeCell ref="F1:F1"/>
+  </mergeCells>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col max="1" min="1" style="2" width="9.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" s="5" customFormat="true"/>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2271,7 +2464,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
feat: Improved esco_service as layer between controller and client
</commit_message>
<xml_diff>
--- a/tests/test_files/handlers/reports/report.xlsx
+++ b/tests/test_files/handlers/reports/report.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Fecha</t>
   </si>
@@ -42,16 +42,16 @@
     <t>-</t>
   </si>
   <si>
+    <t>TASA FIJA</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
     <t>ON HARD DOLLAR</t>
   </si>
   <si>
     <t>RENTA VARIABLE</t>
-  </si>
-  <si>
-    <t>TASA FIJA</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
   </si>
   <si>
     <t>2024-08-01</t>
@@ -61,12 +61,6 @@
   </si>
   <si>
     <t>2024-08-03</t>
-  </si>
-  <si>
-    <t>Tasa de interés de préstamos por adelantos en cuenta corriente</t>
-  </si>
-  <si>
-    <t>Variables de Referencia</t>
   </si>
 </sst>
 </file>
@@ -1938,17 +1932,17 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
@@ -2038,10 +2032,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="E1:E1"/>
+    <mergeCell ref="F1:F1"/>
     <mergeCell ref="B1:B1"/>
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:E1"/>
-    <mergeCell ref="F1:F1"/>
   </mergeCells>
 </worksheet>
 </file>
@@ -2115,17 +2109,17 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
@@ -2264,17 +2258,17 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
@@ -2412,9 +2406,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="B1" s="3"/>
       <c r="C1" s="4"/>
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
@@ -2429,38 +2421,23 @@
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:B1"/>
-  </mergeCells>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
refactor: Changed name voucher for asset
</commit_message>
<xml_diff>
--- a/tests/test_files/handlers/reports/report.xlsx
+++ b/tests/test_files/handlers/reports/report.xlsx
@@ -42,16 +42,16 @@
     <t>-</t>
   </si>
   <si>
+    <t>ON HARD DOLLAR</t>
+  </si>
+  <si>
+    <t>RENTA VARIABLE</t>
+  </si>
+  <si>
     <t>TASA FIJA</t>
   </si>
   <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>ON HARD DOLLAR</t>
-  </si>
-  <si>
-    <t>RENTA VARIABLE</t>
   </si>
   <si>
     <t>2024-08-01</t>
@@ -1932,17 +1932,17 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
@@ -2032,10 +2032,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="B1:B1"/>
+    <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E1"/>
     <mergeCell ref="F1:F1"/>
-    <mergeCell ref="B1:B1"/>
-    <mergeCell ref="C1:D1"/>
   </mergeCells>
 </worksheet>
 </file>
@@ -2109,17 +2109,17 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
@@ -2209,10 +2209,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="B1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E1"/>
     <mergeCell ref="F1:F1"/>
-    <mergeCell ref="B1:B1"/>
   </mergeCells>
 </worksheet>
 </file>
@@ -2258,17 +2258,17 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
@@ -2358,10 +2358,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E1"/>
     <mergeCell ref="F1:F1"/>
+    <mergeCell ref="B1:B1"/>
   </mergeCells>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
feat: added sync log service
</commit_message>
<xml_diff>
--- a/tests/test_files/handlers/reports/report.xlsx
+++ b/tests/test_files/handlers/reports/report.xlsx
@@ -2209,10 +2209,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E1"/>
     <mergeCell ref="F1:F1"/>
+    <mergeCell ref="B1:B1"/>
   </mergeCells>
 </worksheet>
 </file>
@@ -2358,10 +2358,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="B1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E1"/>
     <mergeCell ref="F1:F1"/>
-    <mergeCell ref="B1:B1"/>
   </mergeCells>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
feat: Fixed controller and took out gorm
</commit_message>
<xml_diff>
--- a/tests/test_files/handlers/reports/report.xlsx
+++ b/tests/test_files/handlers/reports/report.xlsx
@@ -42,6 +42,9 @@
     <t>-</t>
   </si>
   <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
     <t>ON HARD DOLLAR</t>
   </si>
   <si>
@@ -49,9 +52,6 @@
   </si>
   <si>
     <t>TASA FIJA</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
   </si>
   <si>
     <t>2024-08-01</t>
@@ -1932,17 +1932,17 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
@@ -2032,10 +2032,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="F1:F1"/>
     <mergeCell ref="B1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E1"/>
-    <mergeCell ref="F1:F1"/>
   </mergeCells>
 </worksheet>
 </file>
@@ -2109,17 +2109,17 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
@@ -2258,17 +2258,17 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>

</xml_diff>

<commit_message>
feat: Improved report as a service
</commit_message>
<xml_diff>
--- a/tests/test_files/handlers/reports/report.xlsx
+++ b/tests/test_files/handlers/reports/report.xlsx
@@ -42,9 +42,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
     <t>ON HARD DOLLAR</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>TASA FIJA</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
   <si>
     <t>2024-08-01</t>
@@ -1932,17 +1932,17 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
@@ -2032,10 +2032,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="F1:F1"/>
     <mergeCell ref="B1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E1"/>
+    <mergeCell ref="F1:F1"/>
   </mergeCells>
 </worksheet>
 </file>
@@ -2109,17 +2109,17 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
@@ -2258,17 +2258,17 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
@@ -2358,10 +2358,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E1"/>
     <mergeCell ref="F1:F1"/>
+    <mergeCell ref="B1:B1"/>
   </mergeCells>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
feat: Refactored account handling to use data from the db
</commit_message>
<xml_diff>
--- a/tests/test_files/handlers/reports/report.xlsx
+++ b/tests/test_files/handlers/reports/report.xlsx
@@ -42,16 +42,16 @@
     <t>-</t>
   </si>
   <si>
+    <t>TASA FIJA</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
     <t>ON HARD DOLLAR</t>
   </si>
   <si>
     <t>RENTA VARIABLE</t>
-  </si>
-  <si>
-    <t>TASA FIJA</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
   </si>
   <si>
     <t>2024-08-01</t>
@@ -1932,17 +1932,17 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
@@ -2032,10 +2032,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="E1:E1"/>
+    <mergeCell ref="F1:F1"/>
     <mergeCell ref="B1:B1"/>
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:E1"/>
-    <mergeCell ref="F1:F1"/>
   </mergeCells>
 </worksheet>
 </file>
@@ -2109,17 +2109,17 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
@@ -2258,17 +2258,17 @@
     <row r="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
@@ -2358,10 +2358,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="E1:E1"/>
+    <mergeCell ref="F1:F1"/>
     <mergeCell ref="B1:B1"/>
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:E1"/>
-    <mergeCell ref="F1:F1"/>
   </mergeCells>
 </worksheet>
 </file>

</xml_diff>